<commit_message>
Initial clean commit for heart segmentation
</commit_message>
<xml_diff>
--- a/example_data/Patient_list/patient_list.xlsx
+++ b/example_data/Patient_list/patient_list.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_0.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_0.nii.gz</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_0.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_0.nii.gz</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -494,12 +494,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_1.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_1.nii.gz</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_1.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_1.nii.gz</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -517,12 +517,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_2.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_2.nii.gz</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_2.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_2.nii.gz</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -540,12 +540,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_3.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_3.nii.gz</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_3.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_3.nii.gz</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -563,12 +563,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_4.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_4.nii.gz</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_4.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_4.nii.gz</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -586,12 +586,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_5.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_5.nii.gz</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_5.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_5.nii.gz</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -609,12 +609,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_6.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_6.nii.gz</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_6.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_6.nii.gz</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -632,12 +632,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_7.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_7.nii.gz</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_7.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_7.nii.gz</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -655,12 +655,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_8.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_8.nii.gz</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_8.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_8.nii.gz</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -678,12 +678,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_9.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_9.nii.gz</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_9.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_9.nii.gz</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -701,12 +701,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_10.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/img/slice_10.nii.gz</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>/host/d/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_10.nii.gz</t>
+          <t>/host/c/Users/Junzhe/Desktop/Whole_heart_segmentation/GitHub/Whole_heart_segmentation_junzhe/example_data/data/ID_0002/seg/slice_10.nii.gz</t>
         </is>
       </c>
       <c r="E12" t="n">

</xml_diff>